<commit_message>
Update Hacker Kermit - Test Protocol Simple ATM Machine.xlsx
</commit_message>
<xml_diff>
--- a/Test Cases/Hacker Kermit - Test Protocol Simple ATM Machine.xlsx
+++ b/Test Cases/Hacker Kermit - Test Protocol Simple ATM Machine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Courses\Sprints\Automotive Software BootCamp\Part 07 - Embedded Systems L2\S_ESL2_CAP_PROJECT_02 Simple ATM Machine\Simple_ATM_Machine\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED044B1-1BFC-4626-AE0F-B87EEDF4A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1290800-081F-4960-B94E-1E2C8AFB9D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,43 +1813,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1880,10 +1843,47 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2205,18 +2205,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="28.5" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="47" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="53" t="s">
         <v>336</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:34" ht="25.5" customHeight="1">
@@ -2235,9 +2235,9 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2266,25 +2266,25 @@
       <c r="AH2" s="4"/>
     </row>
     <row r="3" spans="1:34" ht="15.6">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:34" ht="14.4">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2348,13 +2348,13 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:34" ht="14.4">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2380,13 +2380,13 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:34" ht="14.4">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -2412,35 +2412,35 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:34" ht="14.4">
-      <c r="A12" s="49"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:34" ht="15.6">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:34" ht="14.4">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -2566,13 +2566,13 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="14.4">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2678,13 +2678,13 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="14.4">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2740,25 +2740,25 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="15.6">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="14.4">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2784,13 +2784,13 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:16" ht="14.4">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="45"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="56"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2836,13 +2836,13 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:16" ht="14.4">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2906,13 +2906,13 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:16" ht="15.6">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2987,8 +2987,8 @@
   </sheetPr>
   <dimension ref="A1:Z1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3002,19 +3002,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="73" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -3052,9 +3052,9 @@
       <c r="F2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -3074,14 +3074,14 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -3104,14 +3104,14 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -3137,13 +3137,13 @@
       <c r="A5" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="44" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="29" t="s">
@@ -3157,13 +3157,13 @@
       <c r="A6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="44" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="29" t="s">
@@ -3177,13 +3177,13 @@
       <c r="A7" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="44" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="29" t="s">
@@ -3197,13 +3197,13 @@
       <c r="A8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="44" t="s">
         <v>72</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -3217,13 +3217,13 @@
       <c r="A9" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="44" t="s">
         <v>59</v>
       </c>
       <c r="E9" s="29" t="s">
@@ -3237,13 +3237,13 @@
       <c r="A10" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E10" s="29" t="s">
@@ -3257,13 +3257,13 @@
       <c r="A11" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="44" t="s">
         <v>83</v>
       </c>
       <c r="E11" s="29" t="s">
@@ -3277,13 +3277,13 @@
       <c r="A12" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="44" t="s">
         <v>87</v>
       </c>
       <c r="E12" s="29" t="s">
@@ -3294,14 +3294,14 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="59"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -3327,10 +3327,10 @@
       <c r="A14" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="44" t="s">
         <v>90</v>
       </c>
       <c r="D14" s="35" t="s">
@@ -3367,10 +3367,10 @@
       <c r="A15" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="44" t="s">
         <v>93</v>
       </c>
       <c r="D15" s="35" t="s">
@@ -3407,10 +3407,10 @@
       <c r="A16" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="44" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="35" t="s">
@@ -3447,10 +3447,10 @@
       <c r="A17" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="44" t="s">
         <v>99</v>
       </c>
       <c r="D17" s="35" t="s">
@@ -3487,10 +3487,10 @@
       <c r="A18" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="44" t="s">
         <v>103</v>
       </c>
       <c r="D18" s="35" t="s">
@@ -3524,10 +3524,10 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="45" t="s">
         <v>102</v>
       </c>
       <c r="C19" s="36" t="s">
@@ -3564,14 +3564,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -3597,7 +3597,7 @@
       <c r="A21" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="43" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="28" t="s">
@@ -3637,7 +3637,7 @@
       <c r="A22" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="43" t="s">
         <v>112</v>
       </c>
       <c r="C22" s="28" t="s">
@@ -3677,7 +3677,7 @@
       <c r="A23" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="43" t="s">
         <v>116</v>
       </c>
       <c r="C23" s="28" t="s">
@@ -3714,10 +3714,10 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24" spans="1:26" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="45" t="s">
         <v>119</v>
       </c>
       <c r="C24" s="36" t="s">
@@ -3754,14 +3754,14 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="68"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -3787,10 +3787,10 @@
       <c r="A26" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="44" t="s">
         <v>124</v>
       </c>
       <c r="D26" s="28" t="s">
@@ -3807,10 +3807,10 @@
       <c r="A27" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="44" t="s">
         <v>127</v>
       </c>
       <c r="D27" s="28" t="s">
@@ -3827,10 +3827,10 @@
       <c r="A28" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="44" t="s">
         <v>130</v>
       </c>
       <c r="D28" s="28" t="s">
@@ -3847,10 +3847,10 @@
       <c r="A29" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="43" t="s">
         <v>339</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="44" t="s">
         <v>133</v>
       </c>
       <c r="D29" s="28" t="s">
@@ -3867,10 +3867,10 @@
       <c r="A30" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="44" t="s">
         <v>136</v>
       </c>
       <c r="D30" s="28" t="s">
@@ -3887,10 +3887,10 @@
       <c r="A31" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="43" t="s">
         <v>341</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="44" t="s">
         <v>139</v>
       </c>
       <c r="D31" s="28" t="s">
@@ -3904,26 +3904,26 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="59"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="64"/>
     </row>
     <row r="33" spans="1:6" ht="22.5" customHeight="1">
       <c r="A33" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="43" t="s">
         <v>142</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D33" s="63" t="s">
+      <c r="D33" s="44" t="s">
         <v>144</v>
       </c>
       <c r="E33" s="29" t="s">
@@ -3957,13 +3957,13 @@
       <c r="A35" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="43" t="s">
         <v>150</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="44" t="s">
         <v>152</v>
       </c>
       <c r="E35" s="29" t="s">
@@ -3974,14 +3974,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="59"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="64"/>
     </row>
     <row r="37" spans="1:6" ht="22.5" customHeight="1">
       <c r="A37" s="37" t="s">
@@ -4284,24 +4284,24 @@
       </c>
     </row>
     <row r="52" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A52" s="61" t="s">
+      <c r="A52" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="59"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="64"/>
     </row>
     <row r="53" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="54"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="55"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="68"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -4444,14 +4444,14 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="59"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="64"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -4674,14 +4674,14 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A63" s="57" t="s">
+      <c r="A63" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="59"/>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="64"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -4984,14 +4984,14 @@
       <c r="Z70" s="3"/>
     </row>
     <row r="71" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A71" s="57" t="s">
+      <c r="A71" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B71" s="58"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
-      <c r="F71" s="59"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="63"/>
+      <c r="F71" s="64"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -5214,14 +5214,14 @@
       <c r="Z76" s="3"/>
     </row>
     <row r="77" spans="1:26" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A77" s="57" t="s">
+      <c r="A77" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="58"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="58"/>
-      <c r="F77" s="59"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="64"/>
     </row>
     <row r="78" spans="1:26" ht="22.5" customHeight="1">
       <c r="A78" s="40" t="s">
@@ -5284,24 +5284,24 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A81" s="60" t="s">
+      <c r="A81" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B81" s="51"/>
-      <c r="C81" s="51"/>
-      <c r="D81" s="51"/>
-      <c r="E81" s="51"/>
-      <c r="F81" s="52"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
+      <c r="F81" s="71"/>
     </row>
     <row r="82" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A82" s="57" t="s">
+      <c r="A82" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="58"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="59"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="63"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="63"/>
+      <c r="F82" s="64"/>
     </row>
     <row r="83" spans="1:6" ht="22.5" customHeight="1">
       <c r="A83" s="40" t="s">
@@ -5384,14 +5384,14 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A87" s="57" t="s">
+      <c r="A87" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="59"/>
+      <c r="B87" s="63"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="64"/>
     </row>
     <row r="88" spans="1:6" ht="22.5" customHeight="1">
       <c r="A88" s="40" t="s">
@@ -5594,14 +5594,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A98" s="57" t="s">
+      <c r="A98" s="62" t="s">
         <v>316</v>
       </c>
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="59"/>
+      <c r="B98" s="63"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="64"/>
     </row>
     <row r="99" spans="1:6" ht="22.5" customHeight="1">
       <c r="A99" s="40" t="s">
@@ -5684,22 +5684,22 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A103" s="66" t="s">
+      <c r="A103" s="47" t="s">
         <v>332</v>
       </c>
-      <c r="B103" s="67" t="s">
+      <c r="B103" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="C103" s="68" t="s">
+      <c r="C103" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="D103" s="28" t="s">
+      <c r="D103" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="E103" s="69" t="s">
+      <c r="E103" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="F103" s="70" t="s">
+      <c r="F103" s="51" t="s">
         <v>61</v>
       </c>
     </row>
@@ -8504,6 +8504,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A20:F20"/>
     <mergeCell ref="G1:I2"/>
     <mergeCell ref="A98:F98"/>
     <mergeCell ref="A36:F36"/>
@@ -8520,9 +8523,6 @@
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F12 F14:F19 F21:F24 F26:F31 F33:F35 F37:F51 F54:F56 F58:F62 F64:F70 F72:F76 F83:F86 F88:F97 F99:F103 F78:F80" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>